<commit_message>
also store type of number in FonialNumber
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spossner/PycharmProjects/fonial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianpossner/PycharmProjects/fonial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E5FE9-FA16-DD46-8416-3B5A87B032AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA5A81B-A9C3-C84E-ACAA-9F0541CBE860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="43700" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="36360" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Type</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Admin admin</t>
+  </si>
+  <si>
+    <t>Zoiper</t>
   </si>
 </sst>
 </file>
@@ -529,11 +532,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB95B9D0-6D1A-F448-AAD9-8AADA675BE41}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -546,7 +549,7 @@
     <col min="10" max="10" width="16.5" style="2" customWidth="1"/>
     <col min="11" max="11" width="17.5" style="2" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="2"/>
-    <col min="13" max="13" width="58" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -656,7 +659,7 @@
         <v>DEPLOYED</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I11" si="3">C3</f>
+        <f t="shared" ref="I3:I10" si="3">C3</f>
         <v>Jaqueline Nuernberger</v>
       </c>
       <c r="J3" s="6">
@@ -982,6 +985,34 @@
         <f t="shared" si="2"/>
         <v>NO DEVICE</v>
       </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ref="C13" si="4">A13&amp;" "&amp;B13</f>
+        <v>Arnd Eversberg</v>
+      </c>
+      <c r="D13" s="5">
+        <v>331001007</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" ref="E13" si="5">VALUE(RIGHT(D13,3))</f>
+        <v>7</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f t="shared" ref="H13" si="6">IF(ISTEXT(F13),IF(ISTEXT(K13),"STORAGE",IF(ISTEXT(I13),"DEPLOYED","STORAGE")),"NO DEVICE")</f>
+        <v>NO DEVICE</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="L13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -996,6 +1027,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010043119C1806F90F41A58CFA7527EE0C1D" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2cbe9ea73129eff7ef8a2c48e12c79e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f19b716-678b-450c-820f-797d4ec286ff" xmlns:ns3="a1918404-f406-4db9-8aac-17d9431c041c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9506964deb9fd94747ad5d2a7a75cbc3" ns2:_="" ns3:_="">
     <xsd:import namespace="6f19b716-678b-450c-820f-797d4ec286ff"/>
@@ -1192,15 +1232,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F258792A-B5D9-314E-A104-C079F208AFAE}">
   <ds:schemaRefs>
@@ -1219,6 +1250,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5EEBFB7-CE62-4B94-BF24-6AA8C4055664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC5F46C3-41F9-483F-8C09-9968FDE2940E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1235,12 +1274,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5EEBFB7-CE62-4B94-BF24-6AA8C4055664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>